<commit_message>
Corrección del valor de mutación
</commit_message>
<xml_diff>
--- a/TP3/Resolucion/TablaCapitales.xlsx
+++ b/TP3/Resolucion/TablaCapitales.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Users\R7-Bassi\Desktop\Viajante\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Drive\UTN\5to año - 2020\Trabajos Practicos\Algoritmos Geneticos\TPS-git\TP3\Resolucion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98472B56-0869-4124-B9A9-2A3EB548912E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FFE1763-D15F-43FB-BE50-F8EB6CD9FDDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1351,7 +1351,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>